<commit_message>
add colour prompt to cache lookups table
</commit_message>
<xml_diff>
--- a/cache lookups.xlsx
+++ b/cache lookups.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8712f81eba3c7055/COMP/COMP2310/final/helper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8712f81eba3c7055/COMP/COMP2310/final/ANU-COMP2310-tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_F25DC773A252ABDACC10487B411976065BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1577F603-B25A-4478-BFB8-3F622608AE25}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="11_F25DC773A252ABDACC10487B411976065BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{528C692B-A987-4D31-B842-AC3F55BCF708}"/>
   <bookViews>
-    <workbookView xWindow="-22054" yWindow="-111" windowWidth="22165" windowHeight="13217" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1868" yWindow="5640" windowWidth="16215" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,12 +78,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,8 +104,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -115,6 +122,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -421,16 +432,16 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B2">
-        <v>32</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1">
         <v>1024</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>4</v>
       </c>
       <c r="F2">
@@ -451,16 +462,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B3">
-        <v>32</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="1">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1">
         <v>1024</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>4</v>
       </c>
       <c r="F3">
@@ -481,16 +492,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B4">
-        <v>32</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1">
         <v>1024</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>256</v>
       </c>
       <c r="F4">
@@ -511,16 +522,16 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B5">
-        <v>32</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="1">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1">
         <v>1024</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>8</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5">
@@ -541,16 +552,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B6">
-        <v>32</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1">
         <v>1024</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>8</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>128</v>
       </c>
       <c r="F6">
@@ -571,16 +582,16 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B7">
-        <v>32</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="1">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1">
         <v>1024</v>
       </c>
-      <c r="D7">
-        <v>32</v>
-      </c>
-      <c r="E7">
+      <c r="D7" s="1">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7">
@@ -601,16 +612,16 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B8">
-        <v>32</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="1">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1">
         <v>1024</v>
       </c>
-      <c r="D8">
-        <v>32</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="1">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1">
         <v>4</v>
       </c>
       <c r="F8">

</xml_diff>